<commit_message>
Adding products with numeric values on price column
</commit_message>
<xml_diff>
--- a/main/resources/products.xlsx
+++ b/main/resources/products.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -53,31 +53,19 @@
     <t>Peripherals</t>
   </si>
   <si>
-    <t>350.00</t>
-  </si>
-  <si>
     <t>27" Monitor</t>
   </si>
   <si>
     <t>Monitors</t>
   </si>
   <si>
-    <t>1550.90</t>
-  </si>
-  <si>
     <t>Gaming Mouse</t>
-  </si>
-  <si>
-    <t>220.00</t>
   </si>
   <si>
     <t>Ergonomic Chair</t>
   </si>
   <si>
     <t>Office</t>
-  </si>
-  <si>
-    <t>980.00</t>
   </si>
 </sst>
 </file>
@@ -716,7 +704,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -725,6 +713,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1265,7 +1256,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1304,13 +1295,13 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
+      <c r="D2" s="3">
+        <v>351</v>
       </c>
       <c r="E2" s="2">
         <v>20</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>45667</v>
       </c>
     </row>
@@ -1319,18 +1310,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
+      <c r="D3" s="3">
+        <v>1550.9</v>
       </c>
       <c r="E3" s="2">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>45702</v>
       </c>
     </row>
@@ -1339,18 +1330,18 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
+      <c r="D4" s="3">
+        <v>220</v>
       </c>
       <c r="E4" s="2">
         <v>30</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>45717</v>
       </c>
     </row>
@@ -1359,18 +1350,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>980</v>
       </c>
       <c r="E5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>45767</v>
       </c>
     </row>

</xml_diff>